<commit_message>
Ajuste na exibição da mensagem de sucesso por 2 segundos
</commit_message>
<xml_diff>
--- a/data/relatorio_de_tickets/relatorio_ocorrencias.xlsx
+++ b/data/relatorio_de_tickets/relatorio_ocorrencias.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q763"/>
+  <dimension ref="A1:Q803"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -59766,7 +59766,7 @@
         </is>
       </c>
       <c r="J763" s="2" t="n">
-        <v>45780.05038974131</v>
+        <v>45780.05038974537</v>
       </c>
       <c r="K763" t="inlineStr">
         <is>
@@ -59799,6 +59799,3094 @@
       <c r="Q763" t="inlineStr">
         <is>
           <t>0:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>32455</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D764" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E764" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F764" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G764" t="inlineStr"/>
+      <c r="H764" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I764" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:39:58</t>
+        </is>
+      </c>
+      <c r="J764" s="2" t="n">
+        <v>45780.15276256944</v>
+      </c>
+      <c r="K764" t="inlineStr">
+        <is>
+          <t>rte</t>
+        </is>
+      </c>
+      <c r="L764" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:40:21</t>
+        </is>
+      </c>
+      <c r="M764" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N764" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O764" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P764" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q764" t="inlineStr"/>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>32455</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D765" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E765" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F765" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G765" t="inlineStr"/>
+      <c r="H765" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I765" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:39:58</t>
+        </is>
+      </c>
+      <c r="J765" s="2" t="n">
+        <v>45780.15276256944</v>
+      </c>
+      <c r="K765" t="inlineStr">
+        <is>
+          <t>rte</t>
+        </is>
+      </c>
+      <c r="L765" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:40:21</t>
+        </is>
+      </c>
+      <c r="M765" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N765" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O765" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P765" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q765" t="inlineStr">
+        <is>
+          <t>0:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>32455</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D766" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E766" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F766" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G766" t="inlineStr"/>
+      <c r="H766" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I766" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:39:58</t>
+        </is>
+      </c>
+      <c r="J766" s="2" t="n">
+        <v>45780.15276256944</v>
+      </c>
+      <c r="K766" t="inlineStr">
+        <is>
+          <t>rte</t>
+        </is>
+      </c>
+      <c r="L766" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:40:21</t>
+        </is>
+      </c>
+      <c r="M766" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N766" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O766" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P766" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q766" t="inlineStr">
+        <is>
+          <t>0:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>32455</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D767" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E767" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F767" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G767" t="inlineStr"/>
+      <c r="H767" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I767" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:39:58</t>
+        </is>
+      </c>
+      <c r="J767" s="2" t="n">
+        <v>45780.15276256944</v>
+      </c>
+      <c r="K767" t="inlineStr">
+        <is>
+          <t>rte</t>
+        </is>
+      </c>
+      <c r="L767" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:40:21</t>
+        </is>
+      </c>
+      <c r="M767" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N767" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O767" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P767" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q767" t="inlineStr">
+        <is>
+          <t>0:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D768" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E768" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F768" t="inlineStr">
+        <is>
+          <t>Pedido Bloqueado</t>
+        </is>
+      </c>
+      <c r="G768" t="inlineStr"/>
+      <c r="H768" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I768" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:43:25</t>
+        </is>
+      </c>
+      <c r="J768" s="2" t="n">
+        <v>45780.15515481481</v>
+      </c>
+      <c r="K768" t="inlineStr">
+        <is>
+          <t>23456</t>
+        </is>
+      </c>
+      <c r="L768" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:43:46</t>
+        </is>
+      </c>
+      <c r="M768" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N768" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O768" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P768" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q768" t="inlineStr"/>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>32455</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D769" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E769" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F769" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G769" t="inlineStr"/>
+      <c r="H769" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I769" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:39:58</t>
+        </is>
+      </c>
+      <c r="J769" s="2" t="n">
+        <v>45780.15276256944</v>
+      </c>
+      <c r="K769" t="inlineStr">
+        <is>
+          <t>rte</t>
+        </is>
+      </c>
+      <c r="L769" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:40:21</t>
+        </is>
+      </c>
+      <c r="M769" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N769" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O769" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P769" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q769" t="inlineStr">
+        <is>
+          <t>0:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D770" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E770" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F770" t="inlineStr">
+        <is>
+          <t>Pedido Bloqueado</t>
+        </is>
+      </c>
+      <c r="G770" t="inlineStr"/>
+      <c r="H770" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I770" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:43:25</t>
+        </is>
+      </c>
+      <c r="J770" s="2" t="n">
+        <v>45780.15515481481</v>
+      </c>
+      <c r="K770" t="inlineStr">
+        <is>
+          <t>23456</t>
+        </is>
+      </c>
+      <c r="L770" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:43:46</t>
+        </is>
+      </c>
+      <c r="M770" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N770" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O770" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P770" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q770" t="inlineStr">
+        <is>
+          <t>0:00:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D771" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E771" t="inlineStr">
+        <is>
+          <t>ADALBERTO JOSE MARTINS SOBRINHO</t>
+        </is>
+      </c>
+      <c r="F771" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G771" t="inlineStr"/>
+      <c r="H771" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I771" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:48:47</t>
+        </is>
+      </c>
+      <c r="J771" s="2" t="n">
+        <v>45780.15888113426</v>
+      </c>
+      <c r="K771" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L771" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:15</t>
+        </is>
+      </c>
+      <c r="M771" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N771" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O771" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P771" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q771" t="inlineStr"/>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D772" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E772" t="inlineStr">
+        <is>
+          <t>ADALBERTO JOSE MARTINS SOBRINHO</t>
+        </is>
+      </c>
+      <c r="F772" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G772" t="inlineStr"/>
+      <c r="H772" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I772" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:48:47</t>
+        </is>
+      </c>
+      <c r="J772" s="2" t="n">
+        <v>45780.15888113426</v>
+      </c>
+      <c r="K772" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L772" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:15</t>
+        </is>
+      </c>
+      <c r="M772" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N772" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O772" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P772" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q772" t="inlineStr">
+        <is>
+          <t>0:00:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D773" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E773" t="inlineStr">
+        <is>
+          <t>ADALBERTO JOSE MARTINS SOBRINHO</t>
+        </is>
+      </c>
+      <c r="F773" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G773" t="inlineStr"/>
+      <c r="H773" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I773" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:48:47</t>
+        </is>
+      </c>
+      <c r="J773" s="2" t="n">
+        <v>45780.15888113426</v>
+      </c>
+      <c r="K773" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L773" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:15</t>
+        </is>
+      </c>
+      <c r="M773" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N773" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O773" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P773" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q773" t="inlineStr">
+        <is>
+          <t>0:00:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>23456</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D774" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E774" t="inlineStr">
+        <is>
+          <t>ADALBERTO JOSE MARTINS SOBRINHO</t>
+        </is>
+      </c>
+      <c r="F774" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G774" t="inlineStr"/>
+      <c r="H774" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I774" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:06</t>
+        </is>
+      </c>
+      <c r="J774" s="2" t="n">
+        <v>45780.15909965278</v>
+      </c>
+      <c r="K774" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L774" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:22</t>
+        </is>
+      </c>
+      <c r="M774" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N774" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O774" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P774" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q774" t="inlineStr"/>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D775" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E775" t="inlineStr">
+        <is>
+          <t>ADALBERTO JOSE MARTINS SOBRINHO</t>
+        </is>
+      </c>
+      <c r="F775" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G775" t="inlineStr"/>
+      <c r="H775" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I775" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:48:47</t>
+        </is>
+      </c>
+      <c r="J775" s="2" t="n">
+        <v>45780.15888113426</v>
+      </c>
+      <c r="K775" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L775" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:15</t>
+        </is>
+      </c>
+      <c r="M775" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N775" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O775" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P775" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q775" t="inlineStr">
+        <is>
+          <t>0:00:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>23456</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D776" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E776" t="inlineStr">
+        <is>
+          <t>ADALBERTO JOSE MARTINS SOBRINHO</t>
+        </is>
+      </c>
+      <c r="F776" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G776" t="inlineStr"/>
+      <c r="H776" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I776" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:06</t>
+        </is>
+      </c>
+      <c r="J776" s="2" t="n">
+        <v>45780.15909965278</v>
+      </c>
+      <c r="K776" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L776" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:49:22</t>
+        </is>
+      </c>
+      <c r="M776" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N776" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O776" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P776" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q776" t="inlineStr">
+        <is>
+          <t>0:00:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D777" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E777" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F777" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G777" t="inlineStr"/>
+      <c r="H777" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I777" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:19</t>
+        </is>
+      </c>
+      <c r="J777" s="2" t="n">
+        <v>45780.16134</v>
+      </c>
+      <c r="K777" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="L777" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:32</t>
+        </is>
+      </c>
+      <c r="M777" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N777" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O777" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P777" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q777" t="inlineStr"/>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D778" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E778" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F778" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G778" t="inlineStr"/>
+      <c r="H778" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I778" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:19</t>
+        </is>
+      </c>
+      <c r="J778" s="2" t="n">
+        <v>45780.16134</v>
+      </c>
+      <c r="K778" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="L778" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:32</t>
+        </is>
+      </c>
+      <c r="M778" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N778" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O778" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P778" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q778" t="inlineStr">
+        <is>
+          <t>0:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D779" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E779" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F779" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G779" t="inlineStr"/>
+      <c r="H779" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I779" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:19</t>
+        </is>
+      </c>
+      <c r="J779" s="2" t="n">
+        <v>45780.16134</v>
+      </c>
+      <c r="K779" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="L779" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:32</t>
+        </is>
+      </c>
+      <c r="M779" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N779" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O779" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P779" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q779" t="inlineStr">
+        <is>
+          <t>0:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D780" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E780" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F780" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G780" t="inlineStr"/>
+      <c r="H780" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I780" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:19</t>
+        </is>
+      </c>
+      <c r="J780" s="2" t="n">
+        <v>45780.16134</v>
+      </c>
+      <c r="K780" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="L780" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:32</t>
+        </is>
+      </c>
+      <c r="M780" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N780" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O780" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P780" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q780" t="inlineStr">
+        <is>
+          <t>0:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>4356</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D781" t="inlineStr">
+        <is>
+          <t>rt</t>
+        </is>
+      </c>
+      <c r="E781" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F781" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G781" t="inlineStr"/>
+      <c r="H781" t="inlineStr">
+        <is>
+          <t>ert</t>
+        </is>
+      </c>
+      <c r="I781" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:53:56</t>
+        </is>
+      </c>
+      <c r="J781" s="2" t="n">
+        <v>45780.16246329861</v>
+      </c>
+      <c r="K781" t="inlineStr">
+        <is>
+          <t>4r5t</t>
+        </is>
+      </c>
+      <c r="L781" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:54:02</t>
+        </is>
+      </c>
+      <c r="M781" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N781" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O781" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P781" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q781" t="inlineStr"/>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>AUREA INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D782" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E782" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F782" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G782" t="inlineStr"/>
+      <c r="H782" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I782" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:19</t>
+        </is>
+      </c>
+      <c r="J782" s="2" t="n">
+        <v>45780.16134</v>
+      </c>
+      <c r="K782" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="L782" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:52:32</t>
+        </is>
+      </c>
+      <c r="M782" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N782" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O782" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P782" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q782" t="inlineStr">
+        <is>
+          <t>0:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>4356</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D783" t="inlineStr">
+        <is>
+          <t>rt</t>
+        </is>
+      </c>
+      <c r="E783" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F783" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G783" t="inlineStr"/>
+      <c r="H783" t="inlineStr">
+        <is>
+          <t>ert</t>
+        </is>
+      </c>
+      <c r="I783" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:53:56</t>
+        </is>
+      </c>
+      <c r="J783" s="2" t="n">
+        <v>45780.16246329861</v>
+      </c>
+      <c r="K783" t="inlineStr">
+        <is>
+          <t>4r5t</t>
+        </is>
+      </c>
+      <c r="L783" t="inlineStr">
+        <is>
+          <t>03/05/2025 03:54:02</t>
+        </is>
+      </c>
+      <c r="M783" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N783" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O783" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P783" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q783" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D784" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E784" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F784" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G784" t="inlineStr"/>
+      <c r="H784" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I784" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:02:06</t>
+        </is>
+      </c>
+      <c r="J784" s="2" t="n">
+        <v>45780.16813576389</v>
+      </c>
+      <c r="K784" t="inlineStr">
+        <is>
+          <t>ert</t>
+        </is>
+      </c>
+      <c r="L784" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:02:59</t>
+        </is>
+      </c>
+      <c r="M784" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N784" t="inlineStr"/>
+      <c r="O784" t="inlineStr"/>
+      <c r="P784" t="inlineStr"/>
+      <c r="Q784" t="inlineStr"/>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D785" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E785" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F785" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G785" t="inlineStr"/>
+      <c r="H785" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I785" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:02:06</t>
+        </is>
+      </c>
+      <c r="J785" s="2" t="n">
+        <v>45780.16813576389</v>
+      </c>
+      <c r="K785" t="inlineStr">
+        <is>
+          <t>ert</t>
+        </is>
+      </c>
+      <c r="L785" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:02:59</t>
+        </is>
+      </c>
+      <c r="M785" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="N785" t="inlineStr"/>
+      <c r="O785" t="inlineStr"/>
+      <c r="P785" t="inlineStr"/>
+      <c r="Q785" t="inlineStr">
+        <is>
+          <t>0:00:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>2345</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D786" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E786" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F786" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G786" t="inlineStr"/>
+      <c r="H786" t="inlineStr">
+        <is>
+          <t>bbbbbb</t>
+        </is>
+      </c>
+      <c r="I786" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:08:30</t>
+        </is>
+      </c>
+      <c r="J786" s="2" t="n">
+        <v>45780.17257518518</v>
+      </c>
+      <c r="K786" t="inlineStr">
+        <is>
+          <t>2345678</t>
+        </is>
+      </c>
+      <c r="L786" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:12:19</t>
+        </is>
+      </c>
+      <c r="M786" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N786" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O786" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P786" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q786" t="inlineStr"/>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>21345678</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D787" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E787" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F787" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G787" t="inlineStr"/>
+      <c r="H787" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I787" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:14:31</t>
+        </is>
+      </c>
+      <c r="J787" s="2" t="n">
+        <v>45780.17675660879</v>
+      </c>
+      <c r="K787" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="L787" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:14:39</t>
+        </is>
+      </c>
+      <c r="M787" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N787" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O787" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P787" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q787" t="inlineStr"/>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>21345678</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D788" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E788" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F788" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G788" t="inlineStr"/>
+      <c r="H788" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I788" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:14:31</t>
+        </is>
+      </c>
+      <c r="J788" s="2" t="n">
+        <v>45780.17675660879</v>
+      </c>
+      <c r="K788" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="L788" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:14:39</t>
+        </is>
+      </c>
+      <c r="M788" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N788" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O788" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P788" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q788" t="inlineStr">
+        <is>
+          <t>0:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D789" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E789" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F789" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G789" t="inlineStr"/>
+      <c r="H789" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I789" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J789" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K789" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L789" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:34</t>
+        </is>
+      </c>
+      <c r="M789" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N789" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O789" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P789" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q789" t="inlineStr"/>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D790" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E790" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F790" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G790" t="inlineStr"/>
+      <c r="H790" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I790" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J790" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K790" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L790" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:44</t>
+        </is>
+      </c>
+      <c r="M790" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N790" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O790" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P790" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q790" t="inlineStr"/>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D791" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E791" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F791" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G791" t="inlineStr"/>
+      <c r="H791" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I791" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J791" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K791" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L791" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:53</t>
+        </is>
+      </c>
+      <c r="M791" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N791" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O791" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P791" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q791" t="inlineStr"/>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D792" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E792" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F792" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G792" t="inlineStr"/>
+      <c r="H792" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I792" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J792" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K792" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L792" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:53</t>
+        </is>
+      </c>
+      <c r="M792" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N792" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O792" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P792" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q792" t="inlineStr">
+        <is>
+          <t>0:00:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>erty</t>
+        </is>
+      </c>
+      <c r="D793" t="inlineStr">
+        <is>
+          <t>fgh</t>
+        </is>
+      </c>
+      <c r="E793" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F793" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G793" t="inlineStr"/>
+      <c r="H793" t="inlineStr">
+        <is>
+          <t>fghj</t>
+        </is>
+      </c>
+      <c r="I793" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:19:54</t>
+        </is>
+      </c>
+      <c r="J793" s="2" t="n">
+        <v>45780.18049164352</v>
+      </c>
+      <c r="K793" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="L793" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:23:40</t>
+        </is>
+      </c>
+      <c r="M793" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N793" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O793" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P793" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q793" t="inlineStr"/>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D794" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E794" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F794" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G794" t="inlineStr"/>
+      <c r="H794" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I794" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J794" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K794" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L794" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:53</t>
+        </is>
+      </c>
+      <c r="M794" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N794" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O794" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P794" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q794" t="inlineStr">
+        <is>
+          <t>0:00:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>erty</t>
+        </is>
+      </c>
+      <c r="D795" t="inlineStr">
+        <is>
+          <t>fgh</t>
+        </is>
+      </c>
+      <c r="E795" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F795" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G795" t="inlineStr"/>
+      <c r="H795" t="inlineStr">
+        <is>
+          <t>fghj</t>
+        </is>
+      </c>
+      <c r="I795" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:19:54</t>
+        </is>
+      </c>
+      <c r="J795" s="2" t="n">
+        <v>45780.18049164352</v>
+      </c>
+      <c r="K795" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="L795" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:23:40</t>
+        </is>
+      </c>
+      <c r="M795" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N795" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O795" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P795" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q795" t="inlineStr">
+        <is>
+          <t>0:03:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D796" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E796" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F796" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G796" t="inlineStr"/>
+      <c r="H796" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I796" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J796" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K796" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L796" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:53</t>
+        </is>
+      </c>
+      <c r="M796" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N796" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O796" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P796" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q796" t="inlineStr">
+        <is>
+          <t>0:00:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>erty</t>
+        </is>
+      </c>
+      <c r="D797" t="inlineStr">
+        <is>
+          <t>fgh</t>
+        </is>
+      </c>
+      <c r="E797" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F797" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G797" t="inlineStr"/>
+      <c r="H797" t="inlineStr">
+        <is>
+          <t>fghj</t>
+        </is>
+      </c>
+      <c r="I797" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:19:54</t>
+        </is>
+      </c>
+      <c r="J797" s="2" t="n">
+        <v>45780.18049164352</v>
+      </c>
+      <c r="K797" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="L797" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:23:40</t>
+        </is>
+      </c>
+      <c r="M797" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N797" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O797" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P797" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q797" t="inlineStr">
+        <is>
+          <t>0:03:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D798" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E798" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F798" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G798" t="inlineStr"/>
+      <c r="H798" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I798" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J798" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K798" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L798" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:53</t>
+        </is>
+      </c>
+      <c r="M798" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N798" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O798" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P798" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q798" t="inlineStr">
+        <is>
+          <t>0:00:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>erty</t>
+        </is>
+      </c>
+      <c r="D799" t="inlineStr">
+        <is>
+          <t>fgh</t>
+        </is>
+      </c>
+      <c r="E799" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F799" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G799" t="inlineStr"/>
+      <c r="H799" t="inlineStr">
+        <is>
+          <t>fghj</t>
+        </is>
+      </c>
+      <c r="I799" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:19:54</t>
+        </is>
+      </c>
+      <c r="J799" s="2" t="n">
+        <v>45780.18049164352</v>
+      </c>
+      <c r="K799" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="L799" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:23:40</t>
+        </is>
+      </c>
+      <c r="M799" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N799" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O799" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P799" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q799" t="inlineStr">
+        <is>
+          <t>0:03:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D800" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E800" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F800" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G800" t="inlineStr"/>
+      <c r="H800" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I800" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J800" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K800" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L800" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:53</t>
+        </is>
+      </c>
+      <c r="M800" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N800" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O800" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P800" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q800" t="inlineStr">
+        <is>
+          <t>0:00:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>erty</t>
+        </is>
+      </c>
+      <c r="D801" t="inlineStr">
+        <is>
+          <t>fgh</t>
+        </is>
+      </c>
+      <c r="E801" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F801" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G801" t="inlineStr"/>
+      <c r="H801" t="inlineStr">
+        <is>
+          <t>fghj</t>
+        </is>
+      </c>
+      <c r="I801" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:19:54</t>
+        </is>
+      </c>
+      <c r="J801" s="2" t="n">
+        <v>45780.18049164352</v>
+      </c>
+      <c r="K801" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="L801" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:23:40</t>
+        </is>
+      </c>
+      <c r="M801" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N801" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O801" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P801" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q801" t="inlineStr">
+        <is>
+          <t>0:03:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>34567</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>ffffff</t>
+        </is>
+      </c>
+      <c r="D802" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="E802" t="inlineStr">
+        <is>
+          <t>ADAIR ROBERTO SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="F802" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G802" t="inlineStr"/>
+      <c r="H802" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="I802" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:19</t>
+        </is>
+      </c>
+      <c r="J802" s="2" t="n">
+        <v>45780.17939737268</v>
+      </c>
+      <c r="K802" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="L802" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:18:53</t>
+        </is>
+      </c>
+      <c r="M802" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N802" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O802" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P802" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q802" t="inlineStr">
+        <is>
+          <t>0:00:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>erty</t>
+        </is>
+      </c>
+      <c r="D803" t="inlineStr">
+        <is>
+          <t>fgh</t>
+        </is>
+      </c>
+      <c r="E803" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F803" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G803" t="inlineStr"/>
+      <c r="H803" t="inlineStr">
+        <is>
+          <t>fghj</t>
+        </is>
+      </c>
+      <c r="I803" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:19:54</t>
+        </is>
+      </c>
+      <c r="J803" s="2" t="n">
+        <v>45780.18049164535</v>
+      </c>
+      <c r="K803" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="L803" t="inlineStr">
+        <is>
+          <t>03/05/2025 04:23:40</t>
+        </is>
+      </c>
+      <c r="M803" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N803" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="O803" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="P803" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q803" t="inlineStr">
+        <is>
+          <t>0:03:46</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajustado data/hora abertura e finalização
</commit_message>
<xml_diff>
--- a/data/relatorio_de_tickets/relatorio_ocorrencias.xlsx
+++ b/data/relatorio_de_tickets/relatorio_ocorrencias.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:AN23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,6 +538,106 @@
           <t>Finalizado por</t>
         </is>
       </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>nota_fiscal</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>cliente</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>focal</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>destinatario</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>cidade</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>motorista</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>tipo_de_ocorrencia</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>observacoes</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>responsavel</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>data_hora_abertura</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>abertura_timestamp</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>complementar</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>data_hora_finalizacao</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>cor</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>finalizada</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>finalizado_por</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>tempo_de_permanencia</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>estágio</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -594,7 +694,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O2" t="b">
+      <c r="O2" t="n">
         <v>1</v>
       </c>
       <c r="P2" t="inlineStr">
@@ -610,6 +710,26 @@
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -666,7 +786,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O3" t="b">
+      <c r="O3" t="n">
         <v>1</v>
       </c>
       <c r="P3" t="inlineStr">
@@ -682,6 +802,26 @@
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -738,7 +878,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O4" t="b">
+      <c r="O4" t="n">
         <v>1</v>
       </c>
       <c r="P4" t="inlineStr">
@@ -758,6 +898,26 @@
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -820,7 +980,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O5" t="b">
+      <c r="O5" t="n">
         <v>1</v>
       </c>
       <c r="P5" t="inlineStr">
@@ -844,6 +1004,26 @@
         </is>
       </c>
       <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -906,7 +1086,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O6" t="b">
+      <c r="O6" t="n">
         <v>1</v>
       </c>
       <c r="P6" t="inlineStr">
@@ -930,6 +1110,26 @@
         </is>
       </c>
       <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -992,7 +1192,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O7" t="b">
+      <c r="O7" t="n">
         <v>1</v>
       </c>
       <c r="P7" t="inlineStr">
@@ -1020,6 +1220,26 @@
           <t>rafael</t>
         </is>
       </c>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1082,7 +1302,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O8" t="b">
+      <c r="O8" t="n">
         <v>1</v>
       </c>
       <c r="P8" t="inlineStr">
@@ -1110,6 +1330,26 @@
           <t>rafael</t>
         </is>
       </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1172,7 +1412,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O9" t="b">
+      <c r="O9" t="n">
         <v>1</v>
       </c>
       <c r="P9" t="inlineStr">
@@ -1200,6 +1440,26 @@
           <t>rafael</t>
         </is>
       </c>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1262,7 +1522,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O10" t="b">
+      <c r="O10" t="n">
         <v>1</v>
       </c>
       <c r="P10" t="inlineStr">
@@ -1290,6 +1550,26 @@
           <t>rafael</t>
         </is>
       </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1352,7 +1632,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O11" t="b">
+      <c r="O11" t="n">
         <v>1</v>
       </c>
       <c r="P11" t="inlineStr">
@@ -1380,12 +1660,30 @@
           <t>rafael</t>
         </is>
       </c>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A12" t="n">
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1424,12 +1722,10 @@
         </is>
       </c>
       <c r="J12" s="2" t="n">
-        <v>45783.74732305342</v>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+        <v>45783.74732305556</v>
+      </c>
+      <c r="K12" t="n">
+        <v>33</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1446,7 +1742,7 @@
           <t>#2ecc71</t>
         </is>
       </c>
-      <c r="O12" t="b">
+      <c r="O12" t="n">
         <v>1</v>
       </c>
       <c r="P12" t="inlineStr">
@@ -1474,6 +1770,1252 @@
           <t>rafael</t>
         </is>
       </c>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3333</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>eee</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>vvvv</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>07/05/2025 05:03:36</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>45784.21083795139</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3333</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>07/05/2025 05:03:57</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>0:00:21</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>a45b80a9-aa2d-49df-bfe7-3661e00c2d55</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>SABRINA</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>858f4e0e-99a9-4d1c-845e-ef6c96c0157e</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>555555</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>TRANSPORTADORA KARAVAGGIO LTDA</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>ADELAINE</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>tedte</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>ACIR SEVERO DOS SANTOS</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Pedido Bloqueado</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>2025-05-07 19:33:34</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>2025-05-07 19:33:34</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>te</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>07/05/2025 19:33:59</t>
+        </is>
+      </c>
+      <c r="AI14" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="AK14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AM14" t="inlineStr">
+        <is>
+          <t>Erro ao calcular</t>
+        </is>
+      </c>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>9001a599-a999-42cb-ab34-1b21144284f4</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>66777</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>SABRINA</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>2025-05-07 19:36:56</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>2025-05-07 19:36:56</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>07/05/2025 19:37:18</t>
+        </is>
+      </c>
+      <c r="AI15" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="AK15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AM15" t="inlineStr">
+        <is>
+          <t>Erro ao calcular: can't subtract offset-naive and offset-aware datetimes</t>
+        </is>
+      </c>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>b6925ce0-f5c3-4d65-ba1a-f5e6c599ca54</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>5678</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>IRMAOS RUIVO LTDA-BISCOIT ZEZE</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>PRISCILA</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>ADAILTON VIEIRA</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>2025-05-08 09:15:38</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>2025-05-08 09:15:38</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>08/05/2025 09:16:10</t>
+        </is>
+      </c>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="AK16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AM16" t="inlineStr">
+        <is>
+          <t>Erro ao calcular: can't subtract offset-naive and offset-aware datetimes</t>
+        </is>
+      </c>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>5cc420b9-ff6a-4afe-9621-b06ce6100a2f</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>1235</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>IRMAOS RUIVO LTDA-BISCOIT ZEZE</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>PRISCILA</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>ADAILTON VIEIRA</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Pedido Bloqueado</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>2025-05-08 09:48:09</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>2025-05-08 09:48:09</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>08/05/2025 09:48:33</t>
+        </is>
+      </c>
+      <c r="AI17" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="AK17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AM17" t="inlineStr">
+        <is>
+          <t>Erro ao calcular: can't subtract offset-naive and offset-aware datetimes</t>
+        </is>
+      </c>
+      <c r="AN17" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>750e883e-5ada-4801-9f1b-e3ec25dff609</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
+        <v>2345</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>SABRINA</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>2025-05-08 09:54:20</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>2025-05-08 09:54:20</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>08/05/2025 09:55:26</t>
+        </is>
+      </c>
+      <c r="AI18" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="AK18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AM18" t="inlineStr">
+        <is>
+          <t>Erro ao calcular: can't subtract offset-naive and offset-aware datetimes</t>
+        </is>
+      </c>
+      <c r="AN18" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>498b75a4-cbba-4b76-8e82-e8de6ad701ca</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>34567</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>AXX TRANSPORTES E LOGISTICA LT</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>SABRINA</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>ADAILTON VIEIRA</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>2025-05-08 10:10:37</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>2025-05-08 10:10:37</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>667</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t>08/05/2025 10:11:06</t>
+        </is>
+      </c>
+      <c r="AI19" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="AK19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AM19" t="inlineStr">
+        <is>
+          <t>Erro ao calcular: can't subtract offset-naive and offset-aware datetimes</t>
+        </is>
+      </c>
+      <c r="AN19" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>7a571d7d-cc44-4152-a884-23c5743d422c</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>23345</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>BEBIDAS GRASSI DO BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>JAMILE</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>ACIR SEVERO DOS SANTOS</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>2025-05-08 10:21:56</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>2025-05-08 10:21:56</t>
+        </is>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>4444</t>
+        </is>
+      </c>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>08/05/2025 10:22:19</t>
+        </is>
+      </c>
+      <c r="AI20" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="AK20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="AM20" t="inlineStr">
+        <is>
+          <t>Erro ao calcular: can't subtract offset-naive and offset-aware datetimes</t>
+        </is>
+      </c>
+      <c r="AN20" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>34556</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>AQUAFAST PROD DE LIMPEZA E HIG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ABYNADAB SOARES DINIZ DE CASTRO</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>08/05/2025 10:30:19</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>08/05/2025 10:34:11</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>0:03:52.763537</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>SIMONE</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>6f119353-8446-4430-a505-ce96e48d32b7</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="inlineStr"/>
+      <c r="AK21" t="inlineStr"/>
+      <c r="AL21" t="inlineStr"/>
+      <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TONDO S.A. UN.CACHOERINHA RS</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ABRAO MARTINS PAIXAO</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Pedido Bloqueado</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>08/05/2025 10:39:53</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>08/05/2025 10:39:58</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>gray</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>0:00:05.589056</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>MARIANA</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>b1ad8cbc-f106-416a-acf5-2bc6ecae57a2</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="inlineStr"/>
+      <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="inlineStr"/>
+      <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr">
+        <is>
+          <t>Erro</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ALIANCA EXPRESS TRANSPORTES</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ABNER SABIO SOUZA</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Chegada no Local</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>t3e</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>08/05/2025 21:34:23</t>
+        </is>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>45785.89888136817</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>08/05/2025 21:35:01</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>#2ecc71</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>🟢 Normal</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>0:00:38</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>0d211727-be88-45b6-900b-8f6ef2336fe8</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>SABRINA</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="inlineStr"/>
+      <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr"/>
+      <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>